<commit_message>
chore: save_gpkg and save_shp is updated
</commit_message>
<xml_diff>
--- a/examples/data/direct_analysis/output/hazard_names.xlsx
+++ b/examples/data/direct_analysis/output/hazard_names.xlsx
@@ -463,12 +463,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>maximum</t>
+          <t>average</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>EV1_ma</t>
+          <t>EV1_av</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">

</xml_diff>